<commit_message>
Dragon 5 is now Phönix-1
</commit_message>
<xml_diff>
--- a/Dragon/Dragon_5/Dragon-5.xlsx
+++ b/Dragon/Dragon_5/Dragon-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\user\documents\Nerdshit\processor-development\Dragon\Dragon_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37442C3-2188-4D71-B2EF-F186AABA4932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C8A9C5-2F40-43D9-B3A4-461D87ED3D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15885" activeTab="2" xr2:uid="{8C5D80F7-DE4A-4736-8553-CD227D41FFEF}"/>
+    <workbookView xWindow="38400" yWindow="-8745" windowWidth="14400" windowHeight="16200" activeTab="2" xr2:uid="{8C5D80F7-DE4A-4736-8553-CD227D41FFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" r:id="rId1"/>
@@ -40,8 +40,28 @@
 </workbook>
 </file>
 
+<file path=xl/python.xml><?xml version="1.0" encoding="utf-8"?>
+<python xmlns="http://schemas.microsoft.com/office/spreadsheetml/2023/python">
+  <environmentDefinition id="{882DD1B0-6546-4DFA-8A08-902A380B44EA}">
+    <initialization>
+      <code xml:space="preserve">import numpy as np
+import pandas as pd
+import matplotlib.pyplot as plt
+import seaborn as sns
+import statsmodels as sm
+import excel
+import warnings
+warnings.simplefilter('ignore')
+excel.set_xl_scalar_conversion(excel.convert_to_scalar)
+excel.set_xl_array_conversion(excel.convert_to_dataframe)
+</code>
+    </initialization>
+  </environmentDefinition>
+</python>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="223">
   <si>
     <t>condition</t>
   </si>
@@ -161,12 +181,6 @@
   </si>
   <si>
     <t>OP-Code</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>FLAGS</t>
@@ -355,30 +369,12 @@
     <t>0xf</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
-    <t>DI</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>immediate</t>
   </si>
   <si>
-    <t>RAM</t>
-  </si>
-  <si>
     <t>SOURCE/val</t>
   </si>
   <si>
@@ -550,21 +546,9 @@
     <t>GPR</t>
   </si>
   <si>
-    <t>source register</t>
-  </si>
-  <si>
-    <t>destination register</t>
-  </si>
-  <si>
-    <t>Random Access Memory</t>
-  </si>
-  <si>
     <t>Stack Pointer</t>
   </si>
   <si>
-    <t>Program Pointer</t>
-  </si>
-  <si>
     <t>level input (turing complete)</t>
   </si>
   <si>
@@ -751,15 +735,6 @@
     <t>register B</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>opt: dest reg</t>
   </si>
   <si>
@@ -769,7 +744,49 @@
     <t>zero</t>
   </si>
   <si>
-    <t>Dragon - 1</t>
+    <t>Dragon - 5</t>
+  </si>
+  <si>
+    <t>JaL</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>s0</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>tmp Reg</t>
   </si>
 </sst>
 </file>
@@ -1504,68 +1521,68 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1904,7 +1921,7 @@
   <dimension ref="B2:J64"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,72 +1940,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="59" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
+      <c r="E2" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="58" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
+      <c r="E3" s="77" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="62" t="s">
+      <c r="B5" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="71" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="64"/>
+      <c r="E5" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="73"/>
       <c r="G5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="70" t="s">
-        <v>121</v>
+        <v>66</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="61" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="61"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="72" t="s">
+      <c r="B6" s="70"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="72"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="71"/>
+        <v>85</v>
+      </c>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="76" t="s">
-        <v>161</v>
+      <c r="B7" s="74" t="s">
+        <v>149</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>14</v>
@@ -1997,26 +2014,26 @@
         <v>10</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="77"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
@@ -2024,26 +2041,26 @@
         <v>11</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J8" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="77"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="23" t="s">
         <v>16</v>
       </c>
@@ -2051,80 +2068,80 @@
         <v>12</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="77"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="23" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D10" s="24">
         <v>13</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>92</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="23" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D11" s="29">
         <v>14</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="77"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="23" t="s">
         <v>17</v>
       </c>
@@ -2132,26 +2149,26 @@
         <v>15</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G12" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="77"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="23" t="s">
         <v>18</v>
       </c>
@@ -2159,59 +2176,59 @@
         <v>16</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="77"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="23" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D14" s="24">
         <v>17</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>92</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J14" s="28"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="77"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="23" t="s">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="D15" s="29">
         <v>18</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>38</v>
@@ -2220,132 +2237,132 @@
         <v>38</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="77"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="23" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
       <c r="D16" s="24">
         <v>19</v>
       </c>
       <c r="E16" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="75"/>
+      <c r="C17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="75"/>
+      <c r="C18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="77"/>
-      <c r="C17" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="F18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="75"/>
+      <c r="C19" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E19" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="77"/>
-      <c r="C18" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="24" t="s">
+      <c r="F19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="75"/>
+      <c r="C20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E20" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="77"/>
-      <c r="C19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="77"/>
-      <c r="C20" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="F20" s="26" t="s">
         <v>38</v>
       </c>
@@ -2363,105 +2380,105 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="77"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="78"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>102</v>
-      </c>
       <c r="I22" s="15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="62" t="s">
+      <c r="B25" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="71" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="64"/>
+      <c r="E25" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="73"/>
       <c r="G25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="I25" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="J25" s="70" t="s">
-        <v>121</v>
+        <v>66</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" s="61" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="72" t="s">
+      <c r="B26" s="70"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="72"/>
+      <c r="E26" s="65"/>
       <c r="F26" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="71"/>
+        <v>85</v>
+      </c>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="62"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="73" t="s">
-        <v>160</v>
+      <c r="B27" s="66" t="s">
+        <v>148</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>1</v>
@@ -2470,26 +2487,26 @@
         <v>10</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="74"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="23" t="s">
         <v>2</v>
       </c>
@@ -2497,26 +2514,26 @@
         <v>11</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="74"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="23" t="s">
         <v>3</v>
       </c>
@@ -2524,26 +2541,26 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J29" s="33" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="74"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="23" t="s">
         <v>4</v>
       </c>
@@ -2551,26 +2568,26 @@
         <v>13</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="74"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="23" t="s">
         <v>5</v>
       </c>
@@ -2578,26 +2595,26 @@
         <v>14</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H31" s="32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J31" s="33" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="74"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="23" t="s">
         <v>6</v>
       </c>
@@ -2605,26 +2622,26 @@
         <v>15</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J32" s="28" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="74"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="23" t="s">
         <v>7</v>
       </c>
@@ -2632,26 +2649,26 @@
         <v>16</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H33" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J33" s="33" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="74"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="23" t="s">
         <v>8</v>
       </c>
@@ -2659,26 +2676,26 @@
         <v>17</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="74"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="23" t="s">
         <v>11</v>
       </c>
@@ -2686,26 +2703,26 @@
         <v>18</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J35" s="33" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="74"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="23" t="s">
         <v>9</v>
       </c>
@@ -2713,231 +2730,231 @@
         <v>19</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="74"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J37" s="33" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="74"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="23" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G38" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H38" s="27" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J38" s="28" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="74"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="67"/>
+      <c r="C40" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="67"/>
+      <c r="C41" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I39" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" s="33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="74"/>
-      <c r="C40" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="24" t="s">
+      <c r="E41" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="68"/>
+      <c r="C42" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H40" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="J40" s="28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="74"/>
-      <c r="C41" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="F41" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="H41" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I41" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="J41" s="33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="75"/>
-      <c r="C42" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="E42" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>38</v>
+        <v>91</v>
+      </c>
+      <c r="G42" s="56" t="s">
+        <v>206</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="62" t="s">
+      <c r="B45" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="71" t="s">
         <v>37</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="64"/>
+      <c r="E45" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="73"/>
       <c r="G45" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H45" s="62" t="s">
-        <v>95</v>
-      </c>
-      <c r="I45" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="J45" s="70" t="s">
-        <v>121</v>
+        <v>66</v>
+      </c>
+      <c r="H45" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="I45" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="J45" s="61" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="61"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="72" t="s">
+      <c r="B46" s="70"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="72"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="71"/>
+        <v>85</v>
+      </c>
+      <c r="H46" s="72"/>
+      <c r="I46" s="72"/>
+      <c r="J46" s="62"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="67" t="s">
+      <c r="B47" s="58" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
@@ -2947,26 +2964,26 @@
         <v>10</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G47" s="19" t="s">
         <v>38</v>
       </c>
       <c r="H47" s="36" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="68"/>
+      <c r="B48" s="59"/>
       <c r="C48" s="23" t="s">
         <v>22</v>
       </c>
@@ -2974,26 +2991,26 @@
         <v>11</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G48" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I48" s="37" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J48" s="28" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="68"/>
+      <c r="B49" s="59"/>
       <c r="C49" s="23" t="s">
         <v>23</v>
       </c>
@@ -3001,26 +3018,26 @@
         <v>12</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H49" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I49" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J49" s="33" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="68"/>
+      <c r="B50" s="59"/>
       <c r="C50" s="23" t="s">
         <v>24</v>
       </c>
@@ -3028,26 +3045,26 @@
         <v>13</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F50" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H50" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I50" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="J50" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G50" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H50" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I50" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="J50" s="28" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="51" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="68"/>
+      <c r="B51" s="59"/>
       <c r="C51" s="23" t="s">
         <v>25</v>
       </c>
@@ -3055,26 +3072,26 @@
         <v>14</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F51" s="38" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H51" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="J51" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I51" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="J51" s="33" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="52" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="68"/>
+      <c r="B52" s="59"/>
       <c r="C52" s="23" t="s">
         <v>26</v>
       </c>
@@ -3082,26 +3099,26 @@
         <v>15</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G52" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H52" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I52" s="37" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J52" s="28" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="68"/>
+      <c r="B53" s="59"/>
       <c r="C53" s="23" t="s">
         <v>33</v>
       </c>
@@ -3109,26 +3126,26 @@
         <v>16</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F53" s="38" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H53" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I53" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="68"/>
+      <c r="B54" s="59"/>
       <c r="C54" s="23" t="s">
         <v>36</v>
       </c>
@@ -3136,26 +3153,26 @@
         <v>17</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="F54" s="34" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G54" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H54" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I54" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J54" s="28" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="68"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="23" t="s">
         <v>31</v>
       </c>
@@ -3163,26 +3180,26 @@
         <v>18</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F55" s="38" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G55" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I55" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J55" s="33" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="68"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="23" t="s">
         <v>32</v>
       </c>
@@ -3190,189 +3207,199 @@
         <v>19</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="F56" s="34" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="G56" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H56" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I56" s="37" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J56" s="28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="68"/>
+      <c r="B57" s="59"/>
       <c r="C57" s="23" t="s">
         <v>27</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F57" s="38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G57" s="57" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H57" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I57" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J57" s="33" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="68"/>
+      <c r="B58" s="59"/>
       <c r="C58" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F58" s="34" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G58" s="55" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H58" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I58" s="37" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J58" s="28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="68"/>
+      <c r="B59" s="59"/>
       <c r="C59" s="23" t="s">
         <v>30</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="F59" s="38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G59" s="57" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H59" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I59" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J59" s="33" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="68"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F60" s="34" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G60" s="55" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H60" s="37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I60" s="37" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J60" s="28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="68"/>
+      <c r="B61" s="59"/>
       <c r="C61" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F61" s="38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G61" s="57" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H61" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I61" s="39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J61" s="33" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="69"/>
+      <c r="B62" s="60"/>
       <c r="C62" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G62" s="56" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B47:B62"/>
     <mergeCell ref="J45:J46"/>
     <mergeCell ref="J25:J26"/>
@@ -3389,16 +3416,6 @@
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="B7:B22"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" r:id="rId1"/>
@@ -3410,7 +3427,7 @@
   <dimension ref="B2:F44"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3423,19 +3440,19 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3443,13 +3460,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F3" s="40" t="s">
         <v>38</v>
@@ -3457,13 +3474,13 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>38</v>
@@ -3474,13 +3491,13 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>38</v>
@@ -3494,10 +3511,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>38</v>
@@ -3511,7 +3528,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E7" s="40" t="s">
         <v>38</v>
@@ -3525,7 +3542,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>38</v>
@@ -3536,10 +3553,10 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>38</v>
@@ -3550,13 +3567,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -3564,13 +3581,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -3578,13 +3595,13 @@
         <v>3</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -3592,13 +3609,13 @@
         <v>4</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -3606,13 +3623,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -3620,13 +3637,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -3634,10 +3651,10 @@
         <v>7</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F17" s="40" t="s">
         <v>38</v>
@@ -3648,10 +3665,10 @@
         <v>8</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F18" s="40" t="s">
         <v>38</v>
@@ -3662,13 +3679,13 @@
         <v>11</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -3676,13 +3693,13 @@
         <v>9</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F20" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -3690,13 +3707,13 @@
         <v>10</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -3704,10 +3721,10 @@
         <v>12</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F22" s="40" t="s">
         <v>38</v>
@@ -3718,10 +3735,10 @@
         <v>13</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>38</v>
@@ -3729,13 +3746,13 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="40" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F24" s="40" t="s">
         <v>38</v>
@@ -3743,13 +3760,13 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="40" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F25" s="40" t="s">
         <v>38</v>
@@ -3757,13 +3774,13 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F26" s="40" t="s">
         <v>38</v>
@@ -3774,10 +3791,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>38</v>
@@ -3791,7 +3808,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>38</v>
@@ -3805,7 +3822,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>38</v>
@@ -3819,7 +3836,7 @@
         <v>23</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>38</v>
@@ -3833,7 +3850,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>38</v>
@@ -3847,7 +3864,7 @@
         <v>25</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>38</v>
@@ -3861,7 +3878,7 @@
         <v>26</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E34" s="40" t="s">
         <v>38</v>
@@ -3875,7 +3892,7 @@
         <v>33</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E35" s="40" t="s">
         <v>38</v>
@@ -3889,7 +3906,7 @@
         <v>36</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>38</v>
@@ -3903,7 +3920,7 @@
         <v>31</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E37" s="40" t="s">
         <v>38</v>
@@ -3917,7 +3934,7 @@
         <v>32</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E38" s="40" t="s">
         <v>38</v>
@@ -3931,13 +3948,13 @@
         <v>27</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E39" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F39" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -3945,13 +3962,13 @@
         <v>28</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E40" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -3959,13 +3976,13 @@
         <v>30</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E41" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F41" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -3973,13 +3990,13 @@
         <v>34</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F42" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -3987,13 +4004,13 @@
         <v>29</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E43" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F43" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -4001,13 +4018,13 @@
         <v>35</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4020,7 +4037,7 @@
   <dimension ref="B1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4032,189 +4049,189 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="42" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="51">
         <v>0</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>41</v>
+        <v>212</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>90</v>
+        <v>214</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>88</v>
+        <v>218</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>150</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>151</v>
+        <v>219</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>92</v>
+        <v>220</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>153</v>
+        <v>221</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="47" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>